<commit_message>
Finished initial version of fab files for 12-12 teensy controller arena.
</commit_message>
<xml_diff>
--- a/arena_w_vreg/teensy_arena_12-12/production/version_0p1_r1/CPL_JLCPCB_teensy_arena_12-12_v0p1_r1.xlsx
+++ b/arena_w_vreg/teensy_arena_12-12/production/version_0p1_r1/CPL_JLCPCB_teensy_arena_12-12_v0p1_r1.xlsx
@@ -444,10 +444,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1105,7 +1105,7 @@
         <v>6</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1360,7 +1360,7 @@
         <v>6</v>
       </c>
       <c r="E53" s="2" t="n">
-        <v>0</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1377,7 +1377,7 @@
         <v>6</v>
       </c>
       <c r="E54" s="2" t="n">
-        <v>0</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1394,7 +1394,7 @@
         <v>6</v>
       </c>
       <c r="E55" s="2" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1411,7 +1411,7 @@
         <v>6</v>
       </c>
       <c r="E56" s="2" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1428,7 +1428,7 @@
         <v>6</v>
       </c>
       <c r="E57" s="2" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1436,7 +1436,7 @@
         <v>62</v>
       </c>
       <c r="B58" s="2" t="n">
-        <v>281.659</v>
+        <v>278.659028</v>
       </c>
       <c r="C58" s="2" t="n">
         <v>-196.003</v>
@@ -1445,42 +1445,48 @@
         <v>6</v>
       </c>
       <c r="E58" s="2" t="n">
-        <v>0</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B59" s="2" t="n">
-        <v>276.8461</v>
+        <v>274.247981</v>
       </c>
       <c r="C59" s="2" t="n">
-        <v>-141.6347</v>
+        <v>-143.134745</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E59" s="2" t="n">
-        <v>30</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B60" s="2" t="n">
-        <v>245.4938</v>
+        <v>243.993774</v>
       </c>
       <c r="C60" s="2" t="n">
-        <v>-96.9569</v>
+        <v>-99.555018</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E60" s="2" t="n">
-        <v>60</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
@@ -1490,55 +1496,61 @@
         <v>196.003</v>
       </c>
       <c r="C61" s="2" t="n">
-        <v>-73.941</v>
+        <v>-76.940971</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E61" s="2" t="n">
-        <v>90</v>
-      </c>
+        <v>270</v>
+      </c>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B62" s="2" t="n">
-        <v>141.6347</v>
+        <v>143.134745</v>
       </c>
       <c r="C62" s="2" t="n">
-        <v>-78.7539</v>
+        <v>-81.352018</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E62" s="2" t="n">
-        <v>120</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B63" s="2" t="n">
-        <v>96.9569</v>
+        <v>99.555018</v>
       </c>
       <c r="C63" s="2" t="n">
-        <v>-110.1062</v>
+        <v>-111.606225</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E63" s="2" t="n">
-        <v>150</v>
-      </c>
+        <v>330</v>
+      </c>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B64" s="2" t="n">
-        <v>73.941</v>
+        <v>76.940971</v>
       </c>
       <c r="C64" s="2" t="n">
         <v>-159.597</v>
@@ -1547,42 +1559,48 @@
         <v>6</v>
       </c>
       <c r="E64" s="2" t="n">
-        <v>180</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B65" s="2" t="n">
-        <v>78.7539</v>
+        <v>81.352018</v>
       </c>
       <c r="C65" s="2" t="n">
-        <v>-213.9653</v>
+        <v>-212.465254</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E65" s="2" t="n">
-        <v>-150</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B66" s="2" t="n">
-        <v>110.1062</v>
+        <v>111.606225</v>
       </c>
       <c r="C66" s="2" t="n">
-        <v>-258.6431</v>
+        <v>-256.044981</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E66" s="2" t="n">
-        <v>-120</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
@@ -1592,48 +1610,54 @@
         <v>159.597</v>
       </c>
       <c r="C67" s="2" t="n">
-        <v>-281.659</v>
+        <v>-278.659028</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E67" s="2" t="n">
-        <v>-90</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B68" s="2" t="n">
-        <v>213.9653</v>
+        <v>212.465254</v>
       </c>
       <c r="C68" s="2" t="n">
-        <v>-276.8461</v>
+        <v>-274.247981</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E68" s="2" t="n">
-        <v>-60</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B69" s="2" t="n">
-        <v>258.6431</v>
+        <v>256.044981</v>
       </c>
       <c r="C69" s="2" t="n">
-        <v>-245.4938</v>
+        <v>-243.993774</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E69" s="2" t="n">
-        <v>-30</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">

</xml_diff>